<commit_message>
Update Docs after cadasterimport
</commit_message>
<xml_diff>
--- a/ProjectDocs/jahadurls.xlsx
+++ b/ProjectDocs/jahadurls.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t xml:space="preserve">مسیر</t>
   </si>
@@ -317,7 +317,7 @@
 user.company.is_supernazer</t>
   </si>
   <si>
-    <t xml:space="preserve">/api/landreg/uploadoldcadaster/</t>
+    <t xml:space="preserve">/api/landreg/uploadoldcadasterfromgeodatabase/</t>
   </si>
   <si>
     <r>
@@ -343,6 +343,29 @@
   <si>
     <t xml:space="preserve">فقط superuser , 
 User.company.is_nazer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/landreg/uploadoldcadasterfromshapefile/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ساخت کاداستر قدیمی در دیتابیس برای یک لایه که به صورت 
+شیپ فایل زیپ شده  فرستاده میشود</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/landreg/cadasterimport/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ورود اطلاعات کاداستر قدیمی به جدید از طریق
+مپ کردن ستون ها</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/landreg/colmapvalidate/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">اعتبار سنجی اطلاعات برای مپ شدن بودن تلاش برای ورود به دیتابیس </t>
+  </si>
+  <si>
+    <t xml:space="preserve">/api/landreg/uploadoldcadaster/</t>
   </si>
   <si>
     <r>
@@ -471,7 +494,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -559,8 +582,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="9"/>
+      <sz val="7"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -572,18 +594,30 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="7"/>
+      <sz val="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +698,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFA6"/>
         <bgColor rgb="FFFFF5CE"/>
       </patternFill>
@@ -710,7 +750,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -827,19 +867,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="15" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -898,7 +958,7 @@
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFDE59"/>
-      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF8000"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF77BC65"/>
@@ -1028,8 +1088,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32:A40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="28.35" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1689,7 +1749,7 @@
       <c r="A35" s="6" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="29" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="13" t="s">
@@ -1701,131 +1761,178 @@
       <c r="E35" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="F35" s="29" t="s">
+      <c r="F35" s="30" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="6" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" s="13" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>13</v>
+      <c r="D36" s="32" t="s">
+        <v>54</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" s="29"/>
+        <v>72</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="6" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="24" t="s">
+      <c r="A37" s="33"/>
+      <c r="B37" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E37" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="F37" s="31" t="s">
+      <c r="E37" s="23" t="s">
         <v>74</v>
       </c>
+      <c r="F37" s="30"/>
     </row>
     <row r="38" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="6" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" s="32" t="s">
+      <c r="A38" s="33"/>
+      <c r="B38" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="24" t="s">
+      <c r="C38" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="F38" s="29" t="s">
-        <v>77</v>
-      </c>
+      <c r="F38" s="30"/>
     </row>
     <row r="39" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>75</v>
+        <v>34</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>77</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="29" t="s">
-        <v>77</v>
-      </c>
+      <c r="F39" s="36"/>
     </row>
     <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>79</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="F40" s="29" t="s">
+      <c r="F40" s="36" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="28"/>
+      <c r="A41" s="6" t="n">
+        <v>36</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="A42" s="6" t="n">
+        <v>37</v>
+      </c>
+      <c r="B42" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="36" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="A43" s="6" t="n">
+        <v>38</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
     <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>